<commit_message>
Added Test Data Model
</commit_message>
<xml_diff>
--- a/MobileApp.Automation.Tests/TestData/testData.xlsx
+++ b/MobileApp.Automation.Tests/TestData/testData.xlsx
@@ -155,6 +155,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,7 +427,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>